<commit_message>
sideproject.py added excel added
</commit_message>
<xml_diff>
--- a/foodData123.xlsx
+++ b/foodData123.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김태헌\Desktop\FOODFIGHTER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun-seoyang/Desktop/Welcome./Work/MUNCHERS/MUNCHERS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CF68B5-890B-4971-BB39-A8B43567E324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51204892-6FC3-0245-8F6E-7187F363A14F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3730" yWindow="2420" windowWidth="19200" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mexican" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="131">
   <si>
     <t>id</t>
   </si>
@@ -412,13 +412,21 @@
   </si>
   <si>
     <t>['ketchup', 'worcestershire sauce', 'brown sugar', 'cooked chicken', 'spaghetti', 'chopped green bell pepper', 'chopped onion', 'tomato sauce', 'chili powder']</t>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingredients</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -802,11 +810,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,10 +824,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>18206</v>
       </c>
@@ -828,7 +838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>379</v>
       </c>
@@ -839,7 +849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>28398</v>
       </c>
@@ -850,7 +860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>772</v>
       </c>
@@ -861,7 +871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>30193</v>
       </c>
@@ -872,7 +882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>5241</v>
       </c>
@@ -883,7 +893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>24380</v>
       </c>
@@ -894,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>28751</v>
       </c>
@@ -905,7 +915,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>35076</v>
       </c>
@@ -916,7 +926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>18114</v>
       </c>
@@ -927,7 +937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>31050</v>
       </c>
@@ -938,7 +948,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>32760</v>
       </c>
@@ -949,7 +959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>41721</v>
       </c>
@@ -960,7 +970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>5259</v>
       </c>
@@ -971,7 +981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>41368</v>
       </c>
@@ -982,7 +992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>31536</v>
       </c>
@@ -993,7 +1003,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>22244</v>
       </c>
@@ -1004,7 +1014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>20861</v>
       </c>
@@ -1015,7 +1025,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>47424</v>
       </c>
@@ -1026,7 +1036,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>32102</v>
       </c>
@@ -1049,9 +1059,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>36184</v>
       </c>
@@ -1073,7 +1083,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>20450</v>
       </c>
@@ -1084,7 +1094,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>25054</v>
       </c>
@@ -1095,7 +1105,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>34871</v>
       </c>
@@ -1106,7 +1116,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>79</v>
       </c>
@@ -1117,7 +1127,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>12902</v>
       </c>
@@ -1128,7 +1138,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>22955</v>
       </c>
@@ -1139,7 +1149,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>42007</v>
       </c>
@@ -1150,7 +1160,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>33843</v>
       </c>
@@ -1161,7 +1171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>42295</v>
       </c>
@@ -1172,7 +1182,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>18437</v>
       </c>
@@ -1183,7 +1193,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>4288</v>
       </c>
@@ -1194,7 +1204,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>9132</v>
       </c>
@@ -1205,7 +1215,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>5611</v>
       </c>
@@ -1216,7 +1226,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>42250</v>
       </c>
@@ -1227,7 +1237,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>32725</v>
       </c>
@@ -1238,7 +1248,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>26018</v>
       </c>
@@ -1249,7 +1259,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>30815</v>
       </c>
@@ -1260,7 +1270,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>36419</v>
       </c>
@@ -1271,7 +1281,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>18075</v>
       </c>
@@ -1294,9 +1304,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1307,7 +1317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>35195</v>
       </c>
@@ -1318,7 +1328,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>26340</v>
       </c>
@@ -1329,7 +1339,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>21911</v>
       </c>
@@ -1340,7 +1350,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>11776</v>
       </c>
@@ -1351,7 +1361,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>36514</v>
       </c>
@@ -1362,7 +1372,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>14733</v>
       </c>
@@ -1373,7 +1383,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>20151</v>
       </c>
@@ -1384,7 +1394,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>31925</v>
       </c>
@@ -1395,7 +1405,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>31794</v>
       </c>
@@ -1406,7 +1416,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>31010</v>
       </c>
@@ -1417,7 +1427,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>27722</v>
       </c>
@@ -1428,7 +1438,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>27081</v>
       </c>
@@ -1439,7 +1449,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>1899</v>
       </c>
@@ -1450,7 +1460,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>3414</v>
       </c>
@@ -1461,7 +1471,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>22062</v>
       </c>
@@ -1472,7 +1482,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>43788</v>
       </c>
@@ -1483,7 +1493,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>24682</v>
       </c>
@@ -1494,7 +1504,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>37853</v>
       </c>
@@ -1505,7 +1515,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>18727</v>
       </c>
@@ -1516,7 +1526,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>30705</v>
       </c>
@@ -1537,13 +1547,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1552,7 +1564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>2541</v>
       </c>
@@ -1563,7 +1575,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>942</v>
       </c>
@@ -1574,7 +1586,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>19758</v>
       </c>
@@ -1585,7 +1597,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>39234</v>
       </c>
@@ -1596,7 +1608,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>38212</v>
       </c>
@@ -1607,7 +1619,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>1980</v>
       </c>
@@ -1618,7 +1630,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>43567</v>
       </c>
@@ -1629,7 +1641,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>47372</v>
       </c>
@@ -1640,7 +1652,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>11541</v>
       </c>
@@ -1651,7 +1663,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>11113</v>
       </c>
@@ -1662,7 +1674,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>19540</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>29692</v>
       </c>
@@ -1684,7 +1696,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>20950</v>
       </c>
@@ -1695,7 +1707,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>45513</v>
       </c>
@@ -1706,7 +1718,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>21760</v>
       </c>
@@ -1717,7 +1729,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>19280</v>
       </c>
@@ -1728,7 +1740,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>26955</v>
       </c>
@@ -1739,7 +1751,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>20476</v>
       </c>
@@ -1750,7 +1762,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>10222</v>
       </c>
@@ -1761,7 +1773,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>14473</v>
       </c>
@@ -1782,11 +1794,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1797,7 +1809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>2603</v>
       </c>
@@ -1808,7 +1820,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>30521</v>
       </c>
@@ -1819,7 +1831,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>9411</v>
       </c>
@@ -1830,7 +1842,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4789</v>
       </c>
@@ -1841,7 +1853,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>10757</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>46620</v>
       </c>
@@ -1863,7 +1875,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>24103</v>
       </c>
@@ -1874,7 +1886,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>11159</v>
       </c>
@@ -1885,7 +1897,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>13672</v>
       </c>
@@ -1896,7 +1908,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>46172</v>
       </c>
@@ -1907,7 +1919,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>2408</v>
       </c>
@@ -1918,7 +1930,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>42836</v>
       </c>
@@ -1929,7 +1941,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>19701</v>
       </c>
@@ -1940,7 +1952,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>25229</v>
       </c>
@@ -1951,7 +1963,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>43961</v>
       </c>
@@ -1962,7 +1974,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>40117</v>
       </c>
@@ -1973,7 +1985,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>43270</v>
       </c>
@@ -1984,7 +1996,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>41463</v>
       </c>
@@ -1995,7 +2007,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>43713</v>
       </c>
@@ -2006,7 +2018,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>24621</v>
       </c>
@@ -2029,9 +2041,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2042,7 +2054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>8179</v>
       </c>
@@ -2053,7 +2065,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>3314</v>
       </c>
@@ -2064,7 +2076,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>27561</v>
       </c>
@@ -2075,7 +2087,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>15143</v>
       </c>
@@ -2086,7 +2098,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>3959</v>
       </c>
@@ -2097,7 +2109,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>401</v>
       </c>
@@ -2108,7 +2120,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>3327</v>
       </c>
@@ -2119,7 +2131,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>13500</v>
       </c>
@@ -2130,7 +2142,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>43381</v>
       </c>
@@ -2141,7 +2153,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>21976</v>
       </c>
@@ -2152,7 +2164,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>34706</v>
       </c>
@@ -2163,7 +2175,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>11598</v>
       </c>
@@ -2174,7 +2186,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>46754</v>
       </c>
@@ -2185,7 +2197,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>18384</v>
       </c>
@@ -2196,7 +2208,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>10720</v>
       </c>
@@ -2207,7 +2219,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>28063</v>
       </c>
@@ -2218,7 +2230,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>41566</v>
       </c>
@@ -2229,7 +2241,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>9172</v>
       </c>
@@ -2240,7 +2252,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>34357</v>
       </c>
@@ -2251,7 +2263,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>9392</v>
       </c>

</xml_diff>